<commit_message>
Correcciones sobre el excel de ejecución de casos de prueba
</commit_message>
<xml_diff>
--- a/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
+++ b/Trabajos/Practicos/ISW_2019_4K1_TP12_GRUPO5 - TemplateCasosDePrueba.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezequiel\UTN\Ingenieria de Software\ISW_4K1_GRUPO5_2019\Trabajos\Practicos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Archivos Generales\Facultad\ISW\Repositorio\ISW_4K1_GRUPO5_2019\Trabajos\Practicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655B2258-08F5-479B-8A2A-5DC996C33267}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="679" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
     <sheet name="Bugs" sheetId="28" r:id="rId2"/>
+    <sheet name="Clases_de_Equivalencias" sheetId="29" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Casos_Prueba!$A$9:$AS$2326</definedName>
@@ -23,12 +25,12 @@
     <definedName name="Ready_To_Run">#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr autoRecover="0" repairLoad="1"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="240">
   <si>
     <t>TC_001</t>
   </si>
@@ -421,10 +423,6 @@
     <t>Al ingresar un valor para el campo de "Dirección", éste no es validado por el sistema, así como tampoco genera ningún tipo de aviso en caso que el mismo quede vacío, notificando de la situación.</t>
   </si>
   <si>
-    <t>1. Ingresar un valor alfanumérico (para nombre y para el número de la dirección asociado) al campo "Dirección".
-2. Hacer clic en el botón de "Confirmar Pedido".</t>
-  </si>
-  <si>
     <t>El sistema no aparenta validar el campo "Dirección". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
   </si>
   <si>
@@ -437,10 +435,6 @@
     <t>Al ingresar un valor para el campo de "Referencia Opcional", éste no es validado por el sistema.</t>
   </si>
   <si>
-    <t>1. Ingresar texto en el campo "Referencia Opcional".
-2. Hacer clic en el botón de "Confirmar Pedido".</t>
-  </si>
-  <si>
     <t>Menor</t>
   </si>
   <si>
@@ -448,15 +442,6 @@
   </si>
   <si>
     <t>El sistema no aparenta validar el campo "Monto" al haber seleccionado la opción "Efectivo" para la Forma de Pago elegida. Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
-  </si>
-  <si>
-    <t>1. Seleccionar un valor del menú desplegable de Ciudades.
-2. Hacer clic en el botón de "Confirmar Pedido".</t>
-  </si>
-  <si>
-    <t>1. Seleccionar la opción "Efectivo" del menú desplegable de "Forma de Pago".
-2. Ingresar un monto en el campo de "Monto".
-3. Hacer clic en el botón de "Confirmar Pedido".</t>
   </si>
   <si>
     <t>1. El usuario selecciona la forma de pago "Efectivo".
@@ -483,11 +468,6 @@
   </si>
   <si>
     <t>Al seleccionar la opción "Lo Antes Posible" para el momento de entrega del pedido, y confirmar el mismo, el sistema no hace nada, ni genera ningún tipo de notificación.</t>
-  </si>
-  <si>
-    <t>1. Ingresar un valor válido para la fecha deseada para la recepción del pedido.
-2. Ingresar un valor válido para la hora deseada para la recepción del pedido.
-3. Hacer clic en el botón de "Confirmar Pedido".</t>
   </si>
   <si>
     <t>Los productos iguales no se muestran agrupados.</t>
@@ -564,34 +544,10 @@
 2. El sistema valida que el texto ingresado "Edificio con puerta de vidrio ubicado entre un kiosco y una panadería" sea un texto alfanumérico, o solo texto válido, y lo es.</t>
   </si>
   <si>
-    <t>1. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
-2. Ingresar un número de tarjeta.
-3. Ingresar el nombre y apellido del titular de la tarjeta ingresada.
-4. Ingresar la fecha de vencimiento de la tarjeta ingresada.
-5. Ingresar el código CVC de la tarjeta ingresada.
-6. Hacer clic en el botón de "Confirmar Pedido".</t>
-  </si>
-  <si>
     <t>Al ingresar un valor para los campos "Número de Tarjeta", "Nombre y Apellido", "Fecha de Vencimiento" y "CVC", ninguno es validado por el sistema, así como tampoco genera ningún tipo de aviso en caso que alguno de estos campos queden vacíos, notificando de la situación.</t>
   </si>
   <si>
     <t>El sistema no aparenta validar los campos "Dirección", ni "Ciudad", ni "Fecha Deseada", ni "Hora Deseada", ni "Número de Tarjeta", ni "Nombre y Apellido", ni "Fecha de Vencimiento" ni "CVC". Tampoco muestra ningún mensaje en pantalla avisando de la situación, ni notifica sobre el registro del pedido.</t>
-  </si>
-  <si>
-    <t>1. Ingresar un valor numérico para el campo "Dirección".
-2. No seleccionar ninguna opción para el campo "Ciudad" del menú desplegable de Ciudades.
-3. No seleccionar ninguna opción para el campo "Provincia" del menú desplegable de Provincias.
-4. Ingresar un valor de texto para el campo "ZIP".
-5. Seleccionar la opción "Determinar fecha y hora de recepción".
-6. Ingresar una fecha inválida como fecha de recepción (por ejemplo, anterior a la fecha actual).
-7. Ingresar una hora de recepción.
-8. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
-9. Ingresar un número inválido de tarjeta (por ejemplo, que comienza con '0000').
-10. Ingresar un valor numérico como nombre del titular de la tarjeta.
-11. Ingresar un valor numérico como apellido del titular de la tarjeta.
-12. Ingresar una fecha anterior a la fecha actual como fecha de vencimiento de la tarjeta.
-13. Ingresar un código CVC inválido (por ejemplo, '0').
-14. Seleccionar la opción "Aceptar".</t>
   </si>
   <si>
     <t>Grupo 5</t>
@@ -656,30 +612,258 @@
 6. El usuario selecciona la opcion "Aceptar"</t>
   </si>
   <si>
+    <t>Condición Externa</t>
+  </si>
+  <si>
+    <t>Clases de Equivalencia Validas</t>
+  </si>
+  <si>
+    <t>Clases de Equivalencia Invalidas</t>
+  </si>
+  <si>
+    <t>Clases de Equivalencia de Entradas</t>
+  </si>
+  <si>
+    <t>Número de calle positivo y existente. Nombre de calle existente.</t>
+  </si>
+  <si>
+    <t>Número de calle negativo o inexistente, nombre de calle existente.</t>
+  </si>
+  <si>
+    <t>Número de calle positivo y existente, nombre de calle inexistente.</t>
+  </si>
+  <si>
+    <t>Número de calle negativo o inexistente, nombre de calle inexistente.</t>
+  </si>
+  <si>
+    <t>No ingreso de datos.</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Una selección valida del listado de ciudades disponibles.</t>
+  </si>
+  <si>
+    <t>No selecciona del listado de ciudades disponibles.</t>
+  </si>
+  <si>
+    <t>Ingrese texto.</t>
+  </si>
+  <si>
+    <t>No ingrese texto.</t>
+  </si>
+  <si>
+    <t>Forma de Pago: Efectivo</t>
+  </si>
+  <si>
+    <t>Número positivo mayor o igual al monto del pedido.</t>
+  </si>
+  <si>
+    <t>Número negativo.</t>
+  </si>
+  <si>
+    <t>Número menor al monto del pedido.</t>
+  </si>
+  <si>
+    <t>Ingresa caracteres no numéricos.</t>
+  </si>
+  <si>
+    <t>No ingresa valor.</t>
+  </si>
+  <si>
+    <t>Forma de Pago: Tarjeta VISA</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, Nombre y Apellido del titular válido, fecha de vencimiento válido, CVC válido.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA no existe.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta que no sea VISA.</t>
+  </si>
+  <si>
+    <t>Longitud de número de tarjeta inválida.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, Nombre y Apellido del titular no coincide o no existe.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, ingresa caracteres numéricos en nombre y Apellido del Titular.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, no ingresa datos del nombre de apellido y nombre del Titular.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, Nombre y Apellido del titular válido, Fecha de vencimiento menor al mes de la fecha actual (Tarjeta Vencida).</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, Nombre y Apellido del titular válido, ingresa caracteres no numéricos en la fecha de vencimiento.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, Nombre y Apellido del titular válido, no ingresa fecha de vencimiento.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, Nombre y Apellido del titular válido, fecha de vencimiento válido, número de CVC no es correcto.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, Nombre y Apellido del titular válido, fecha de vencimiento válido, número de CVC no ingresado.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, Nombre y Apellido del titular válido, fecha de vencimiento válido, longitud de número de CVC es incorrecto.</t>
+  </si>
+  <si>
+    <t>Número de tarjeta VISA válido, Nombre y Apellido del titular válido, fecha de vencimiento válido, ingreso de caracteres no numéricos en número de CVC.</t>
+  </si>
+  <si>
+    <t>Selecciona la opción.</t>
+  </si>
+  <si>
+    <t>No selecciona la opción.</t>
+  </si>
+  <si>
+    <t>Fecha y hora valida,  posterior a la fecha actual.</t>
+  </si>
+  <si>
+    <t>Fecha y hora de entrega no válida.</t>
+  </si>
+  <si>
+    <t>Fecha y hora de entrega anterior a la fecha actual.</t>
+  </si>
+  <si>
+    <t>No ingresa fecha y hora de entrega.</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Esté logueado y de rol de comprador.</t>
+  </si>
+  <si>
+    <t>No está logueado.</t>
+  </si>
+  <si>
+    <t>Está logueado y tiene otro rol.</t>
+  </si>
+  <si>
+    <t>Clases de equivalencia de Salidas</t>
+  </si>
+  <si>
+    <t>Debe contener al menos un producto, y el producto debe ser del comercio adherido seleccionado.</t>
+  </si>
+  <si>
+    <t>No contiene ningún producto.</t>
+  </si>
+  <si>
+    <t>El producto no existe.</t>
+  </si>
+  <si>
+    <t>El producto no pertenece al comercio adherido seleccionado.</t>
+  </si>
+  <si>
+    <t>Fecha y hora válidas, posterior a la fecha actual.</t>
+  </si>
+  <si>
+    <t>Fecha y hora estimada de entrega anterior a la fecha actual.</t>
+  </si>
+  <si>
+    <t>No ingresa fecha y hora estimada de entrega.</t>
+  </si>
+  <si>
+    <t>Momento de Entrega: Lo Antes Posible</t>
+  </si>
+  <si>
+    <t>Momento de Entrega: Fecha y Hora de Recepción</t>
+  </si>
+  <si>
+    <t>Provincia</t>
+  </si>
+  <si>
+    <t>Una selección valida del listado de provincias disponibles.</t>
+  </si>
+  <si>
+    <t>No selecciona del listado de provincias disponibles.</t>
+  </si>
+  <si>
+    <t>Código Postal</t>
+  </si>
+  <si>
+    <t>Número positivo mayor a cero, y existente.</t>
+  </si>
+  <si>
+    <t>Código postal negativo o  inexistente.</t>
+  </si>
+  <si>
+    <t>1. Ingresar el valor alfanumérico (para nombre y para el número de la dirección asociado) "Bv. Illia 430" al campo "Dirección".
+2. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>1. Seleccionar el valor "Córdoba" del menú desplegable de Ciudades.
+2. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>1. Ingresar el texto "Edificio con puerta de vidrio ubicado entre un kiosco y una panadería" en el campo "Referencia Opcional".
+2. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción "Efectivo" del menú desplegable de "Forma de Pago", al haber generado un pedido con un monto total de $450.
+2. Ingresar el monto "400" en el campo de "Monto".
+3. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
+2. Ingresar el número de tarjeta "4755 1234 5678 9012".
+3. Ingresar el nombre y apellido del titular "Agustín Rodriguez" de la tarjeta ingresada.
+4. Ingresar la fecha de vencimiento "05/20" de la tarjeta ingresada.
+5. Ingresar el código CVC "598" de la tarjeta ingresada.
+6. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>1. Ingresar el valor "15/10/2019" para la fecha deseada para la recepción del pedido.
+2. Ingresar el valor "22:00" para la hora deseada para la recepción del pedido.
+3. Hacer clic en el botón de "Confirmar Pedido".</t>
+  </si>
+  <si>
+    <t>1. Ingresar el valor numérico "598" para el campo "Dirección".
+2. No seleccionar ninguna opción para el campo "Ciudad" del menú desplegable de Ciudades.
+3. No seleccionar ninguna opción para el campo "Provincia" del menú desplegable de Provincias.
+4. Ingresar el valor de texto "aaa" para el campo "ZIP".
+5. Seleccionar la opción "Determinar fecha y hora de recepción".
+6. Ingresar la fecha "15/09/2019" como fecha de recepción (por ejemplo, anterior a la fecha actual).
+7. Ingresar la hora de recepción "22:00".
+8. Seleccionar la opción "Pago con Tarjeta VISA" del menú desplegable de "Forma de Pago".
+9. Ingresar el número de tarjeta "0000 1111 2222 3333".
+10. Ingresar el valor "156" como nombre y apellido del titular de la tarjeta.
+11. Ingresar la fecha "04/17" como fecha de vencimiento de la tarjeta.
+12. Ingresar el código CVC "0".
+13. Seleccionar la opción "Aceptar".</t>
+  </si>
+  <si>
+    <t>1. Seleccionar la opción "Determinar fecha y hora de recepción".
+2. Ingresar la fecha de recepcion "10/14/2019".
+3. Ingresar la hora de recepcion "35:20".
+4. Seleccionar la opcion de forma de pago "Efectivo".
+5. Ingresar el numero "-300" para el monto de pago.
+6. Seleccionar la opcion "Aceptar".</t>
+  </si>
+  <si>
     <t>1. El sistema valida que el usuario haya seleccionado una opción de momento de entrega, y es así.
 2. El sistema valida que la fecha ingresada por el usuario "10/14/2019" sea una fecha con formato válido, mayor o igual a la fecha actual, y no es así.
 3. El sistema valida que la hora ingresada por el usuario "35:20" sea una hora con formato válido, mayor a la hora actual, y no es así.
 4. El sistema valida que el usuario haya seleccionado una opción de forma de pago, y es así.
 5. El sistema valida que el monto ingresado "-300"  sea mayor o igual al monto del pedio o si es un numero negativo, y no es asi.
-6. El sistema muestra mensaje de "Datos Erroneos"</t>
-  </si>
-  <si>
-    <t>1. Seleccionar la opción "Determinar fecha y hora de recepción".
-2. Ingresar una fecha de recepcion con formato "MM/DD/AAA"  y que sea menor a la actual.
-3. Ingresar la hora de recepcion con formato "MM:HH".
-4. Seleccionar la opcion de forma de pago "Efectivo".
-5. Ingresar un numero negativo para el monto de pago.
-6. Seleccionar la opcion "Aceptar".</t>
+6. El sistema muestra mensaje de "Datos Erróneos"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -788,8 +972,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,8 +1064,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1050,6 +1264,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1067,7 +1381,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1200,17 +1514,59 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="DataPilot Category" xfId="1"/>
-    <cellStyle name="DataPilot Corner" xfId="2"/>
-    <cellStyle name="DataPilot Field" xfId="3"/>
-    <cellStyle name="DataPilot Result" xfId="4"/>
-    <cellStyle name="DataPilot Title" xfId="5"/>
-    <cellStyle name="DataPilot Value" xfId="6"/>
+    <cellStyle name="DataPilot Category" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="DataPilot Corner" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="DataPilot Field" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="DataPilot Result" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="DataPilot Title" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="DataPilot Value" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="8"/>
+    <cellStyle name="Normal 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Total" xfId="9" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="116">
@@ -2497,15 +2853,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AS68"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2674,10 +3030,10 @@
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="43" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E5" s="52"/>
       <c r="F5" s="53"/>
@@ -2888,7 +3244,7 @@
         <v>115</v>
       </c>
       <c r="J11" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K11" s="29">
         <v>1</v>
@@ -2921,19 +3277,19 @@
         <v>86</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E12" s="26" t="s">
         <v>83</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H12" s="26" t="s">
         <v>116</v>
@@ -2942,7 +3298,7 @@
         <v>115</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="K12" s="29">
         <v>2</v>
@@ -2987,7 +3343,7 @@
         <v>89</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H13" s="26" t="s">
         <v>116</v>
@@ -2996,7 +3352,7 @@
         <v>115</v>
       </c>
       <c r="J13" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K13" s="29">
         <v>3</v>
@@ -3029,7 +3385,7 @@
         <v>80</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>90</v>
+        <v>184</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>91</v>
@@ -3038,10 +3394,10 @@
         <v>93</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H14" s="26" t="s">
         <v>116</v>
@@ -3050,7 +3406,7 @@
         <v>115</v>
       </c>
       <c r="J14" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K14" s="29">
         <v>4</v>
@@ -3083,7 +3439,7 @@
         <v>80</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>90</v>
+        <v>190</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>94</v>
@@ -3104,7 +3460,7 @@
         <v>115</v>
       </c>
       <c r="J15" s="28" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K15" s="29">
         <v>5</v>
@@ -3158,7 +3514,7 @@
         <v>115</v>
       </c>
       <c r="J16" s="28" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K16" s="29">
         <v>6</v>
@@ -3212,7 +3568,7 @@
         <v>115</v>
       </c>
       <c r="J17" s="28" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K17" s="29">
         <v>7</v>
@@ -3254,7 +3610,7 @@
         <v>111</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G18" s="26" t="s">
         <v>114</v>
@@ -3266,7 +3622,7 @@
         <v>115</v>
       </c>
       <c r="J18" s="28" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="K18" s="29">
         <v>8</v>
@@ -3308,19 +3664,19 @@
         <v>110</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G19" s="26" t="s">
         <v>112</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I19" s="15" t="s">
         <v>115</v>
       </c>
       <c r="J19" s="28" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="K19" s="29">
         <v>9</v>
@@ -3356,25 +3712,25 @@
         <v>106</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E20" s="26" t="s">
         <v>110</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H20" s="26" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>115</v>
       </c>
       <c r="J20" s="28" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="K20" s="29">
         <v>9</v>
@@ -3410,16 +3766,16 @@
         <v>90</v>
       </c>
       <c r="D21" s="45" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G21" s="26" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H21" s="26" t="s">
         <v>116</v>
@@ -3464,31 +3820,31 @@
         <v>95</v>
       </c>
       <c r="D22" s="45" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E22" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="F22" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="H22" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="F22" s="67" t="s">
+        <v>169</v>
+      </c>
+      <c r="G22" s="67" t="s">
+        <v>239</v>
+      </c>
+      <c r="H22" s="67" t="s">
         <v>116</v>
       </c>
       <c r="I22" s="46" t="s">
         <v>115</v>
       </c>
       <c r="J22" s="28" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="K22" s="29">
         <v>11</v>
       </c>
       <c r="L22" s="37" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="M22" s="39"/>
       <c r="N22" s="15"/>
@@ -4980,7 +5336,7 @@
       <c r="AS68" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:AS2326"/>
+  <autoFilter ref="A9:AS2326" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A2:F4"/>
     <mergeCell ref="H8:L8"/>
@@ -5409,12 +5765,12 @@
       <formula>"Can't Run"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
-    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P62:P63 K62:K63 U62:U63"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I23:I68 S11:S68 N11:N68 I11:I21">
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P62:P63 K62:K63 U62:U63" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I23:I68 S11:S68 N11:N68 I11:I21" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pendiente de Ejecución,Paso,Fallo,Bloqueado,No aplica"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B23:B68 B15:B21">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B23:B68 B15:B21" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5425,11 +5781,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5501,7 +5857,7 @@
         <v>121</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>122</v>
+        <v>231</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>118</v>
@@ -5524,10 +5880,10 @@
         <v>43753</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>131</v>
+        <v>232</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>118</v>
@@ -5539,7 +5895,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
         <v>3</v>
       </c>
@@ -5550,13 +5906,13 @@
         <v>43753</v>
       </c>
       <c r="D6" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>126</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>128</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>104</v>
@@ -5576,10 +5932,10 @@
         <v>43753</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>132</v>
+        <v>234</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>118</v>
@@ -5591,7 +5947,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="108" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="132" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
         <v>5</v>
       </c>
@@ -5602,10 +5958,10 @@
         <v>43753</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>162</v>
+        <v>235</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>118</v>
@@ -5628,10 +5984,10 @@
         <v>43753</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>118</v>
@@ -5654,10 +6010,10 @@
         <v>43753</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>140</v>
+        <v>236</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>118</v>
@@ -5680,13 +6036,13 @@
         <v>43753</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>86</v>
@@ -5706,10 +6062,10 @@
         <v>43753</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F12" s="21" t="s">
         <v>118</v>
@@ -5721,7 +6077,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="288" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="276" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>10</v>
       </c>
@@ -5732,10 +6088,10 @@
         <v>43753</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>165</v>
+        <v>237</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>118</v>
@@ -5747,21 +6103,21 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="120" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="84" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
         <v>11</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C14" s="44">
         <v>43753</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>178</v>
+        <v>238</v>
       </c>
       <c r="F14" s="21" t="s">
         <v>118</v>
@@ -5823,13 +6179,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Bloqueante,Critico,Severo,Menor,Cosmetico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Creado,En Desarrollo,En Prueba,Resuelto,Bloqueado,Cancelado,Cerrado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5837,24 +6193,398 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52429422-1CEF-4B7F-91FA-6FEDF801C0FB}">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="63.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="61"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="56" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="61"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="63"/>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="63"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="56" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
+        <v>225</v>
+      </c>
+      <c r="B9" s="56" t="s">
+        <v>226</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="56"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="62"/>
+    </row>
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="63"/>
+      <c r="B13" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" s="63"/>
+    </row>
+    <row r="14" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="62" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="61"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="56" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="61"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="56" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="63"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="56" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="62" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="61"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="56" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="56" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="61"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="56" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="61"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="56" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="61"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="56" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="61"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="56" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="61"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="56" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="61"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="56" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="61"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="56" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="61"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="56" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="61"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="56" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="63"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="56" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="57" t="s">
+        <v>223</v>
+      </c>
+      <c r="B31" s="56" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="62" t="s">
+        <v>224</v>
+      </c>
+      <c r="B32" s="62" t="s">
+        <v>207</v>
+      </c>
+      <c r="C32" s="56" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="61"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="56" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="63"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="56" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="62" t="s">
+        <v>211</v>
+      </c>
+      <c r="B35" s="62" t="s">
+        <v>212</v>
+      </c>
+      <c r="C35" s="56" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="63"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="56" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="B37" s="59"/>
+      <c r="C37" s="60"/>
+    </row>
+    <row r="38" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="62" t="s">
+        <v>216</v>
+      </c>
+      <c r="C38" s="56" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="61"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="56" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="63"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="56" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="62" t="s">
+        <v>220</v>
+      </c>
+      <c r="C41" s="56" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="61"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="56" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="63"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="56" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A18:A30"/>
+    <mergeCell ref="B18:B30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -5980,25 +6710,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6014,4 +6743,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>